<commit_message>
Redesigned the interface, added a menu bar.
</commit_message>
<xml_diff>
--- a/Tests/Window Layout.xlsx
+++ b/Tests/Window Layout.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Desktop\Python\Projetos\CIE Chromaticity\Tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9e8c9bfceb7de713/Documentos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2240522D-509A-46F4-B14B-86F4179ADA29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{0175EB05-10FA-4DEB-B00D-B593EB8D5B43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{EAFB3CA0-3571-4049-BB89-B21D3AD28453}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{172AA20B-51F1-427A-A2A8-55E096F8C03C}"/>
   </bookViews>
@@ -40,9 +40,6 @@
     <t>Toolbar</t>
   </si>
   <si>
-    <t>Load / Clear buttons</t>
-  </si>
-  <si>
     <t>Color info</t>
   </si>
   <si>
@@ -71,6 +68,9 @@
   </si>
   <si>
     <t>#ffffff</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Spectral distribution</t>
   </si>
 </sst>
 </file>
@@ -94,7 +94,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -102,23 +102,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -436,7 +484,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D068FC-8FA5-4579-BB87-DBCB1B539A3E}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -445,30 +495,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -476,11 +525,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E97E141-C6F0-4BCA-AEB0-02F02CF8E838}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -489,47 +536,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:C5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>